<commit_message>
update naar 1.1.0 en reparaties
</commit_message>
<xml_diff>
--- a/results/result02082021-11-12_excel.xls.xlsx
+++ b/results/result02082021-11-12_excel.xls.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E8E4056-BB89-4A85-9AB0-73206665B56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A69AE3-99D0-4FA8-A48A-93B94DC584CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validatie-terugmeldingen" sheetId="1" r:id="rId1"/>
     <sheet name="Filterbaar Validatie-Resultaat" sheetId="2" r:id="rId2"/>
     <sheet name="Validatie-rapport" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4020,7 +4031,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4881,10 +4892,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1999" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -19280,12 +19293,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F986"/>
   <sheetViews>
-    <sheetView topLeftCell="A667" workbookViewId="0"/>
+    <sheetView topLeftCell="A493" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -37678,7 +37694,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>